<commit_message>
Added Appendix(for real this time ;) ) and wrote to senarios
</commit_message>
<xml_diff>
--- a/Rapport/Plan.xlsx
+++ b/Rapport/Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
   <si>
     <t>What to do?</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Første prototype (MEGET skrapet)</t>
   </si>
   <si>
-    <t>Feedback af prototype</t>
-  </si>
-  <si>
     <t>Første udkast af rapport</t>
   </si>
   <si>
@@ -109,6 +106,15 @@
   </si>
   <si>
     <t>S/R/E</t>
+  </si>
+  <si>
+    <t>2. Interview af lærere på AT</t>
+  </si>
+  <si>
+    <t>Feedback af prototype 1</t>
+  </si>
+  <si>
+    <t>Feedback af prototype 2</t>
   </si>
 </sst>
 </file>
@@ -674,13 +680,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -984,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,16 +1046,16 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="61"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
+      <c r="E2" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -1063,10 +1069,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>15</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="31"/>
@@ -1082,10 +1088,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="4"/>
@@ -1098,16 +1104,16 @@
       <c r="K4" s="14"/>
       <c r="L4" s="4"/>
       <c r="M4" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N4" s="21"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="22"/>
@@ -1120,16 +1126,16 @@
       <c r="K5" s="13"/>
       <c r="L5" s="22"/>
       <c r="M5" s="27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N5" s="28"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="22"/>
@@ -1143,15 +1149,15 @@
       <c r="L6" s="22"/>
       <c r="M6" s="13"/>
       <c r="N6" s="28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>14</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="22"/>
@@ -1165,7 +1171,7 @@
       <c r="L7" s="22"/>
       <c r="M7" s="27"/>
       <c r="N7" s="28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1202,16 +1208,16 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="46"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
+      <c r="E10" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1222,14 +1228,14 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" s="30"/>
       <c r="F11" s="31"/>
@@ -1247,11 +1253,11 @@
         <v>5</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" s="32"/>
       <c r="F12" s="29"/>
@@ -1269,11 +1275,11 @@
         <v>4</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" s="30"/>
       <c r="F13" s="31"/>
@@ -1291,11 +1297,11 @@
         <v>6</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="29"/>
@@ -1310,10 +1316,10 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="7"/>
@@ -1322,7 +1328,7 @@
       <c r="G15" s="48"/>
       <c r="H15" s="7"/>
       <c r="I15" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="8"/>
@@ -1332,10 +1338,10 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="4"/>
@@ -1343,10 +1349,10 @@
       <c r="F16" s="29"/>
       <c r="G16" s="32"/>
       <c r="H16" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I16" s="35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="14"/>
@@ -1359,7 +1365,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="22"/>
@@ -1367,10 +1373,10 @@
       <c r="F17" s="31"/>
       <c r="G17" s="30"/>
       <c r="H17" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I17" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J17" s="22"/>
       <c r="K17" s="13"/>
@@ -1380,10 +1386,10 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="49"/>
@@ -1392,8 +1398,8 @@
       <c r="G18" s="42"/>
       <c r="H18" s="49"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="64" t="s">
-        <v>18</v>
+      <c r="J18" s="62" t="s">
+        <v>17</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="49"/>
@@ -1401,7 +1407,9 @@
       <c r="N18" s="50"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
+      <c r="A19" s="43" t="s">
+        <v>30</v>
+      </c>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="7"/>
@@ -1417,7 +1425,9 @@
       <c r="N19" s="51"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="B20" s="5"/>
       <c r="C20" s="2"/>
       <c r="D20" s="5"/>
@@ -1482,16 +1492,16 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="46"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="63"/>
-      <c r="G24" s="63"/>
+      <c r="E24" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1505,7 +1515,7 @@
         <v>7</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="22"/>
@@ -1513,10 +1523,10 @@
       <c r="F25" s="31"/>
       <c r="G25" s="30"/>
       <c r="H25" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I25" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J25" s="22"/>
       <c r="K25" s="13"/>
@@ -1526,10 +1536,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="22"/>
@@ -1539,7 +1549,7 @@
       <c r="H26" s="24"/>
       <c r="I26" s="13"/>
       <c r="J26" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K26" s="13"/>
       <c r="L26" s="22"/>
@@ -1548,10 +1558,10 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="4"/>

</xml_diff>